<commit_message>
Edit Mp -> Cmp
</commit_message>
<xml_diff>
--- a/Xlsx/Source/ActorBodyPart.xlsx
+++ b/Xlsx/Source/ActorBodyPart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godo\Drafts\Franken\Xlsx\Source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Franken\Xlsx\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A464715-2E25-4922-9C5E-CD71E1E83777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDAE94A6-BAB2-4754-AF01-DD0D668D1323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,10 +95,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mp</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Pt</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -231,6 +227,10 @@
   </si>
   <si>
     <t>Quality</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cmp</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -681,7 +681,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -729,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -740,16 +740,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -796,190 +796,190 @@
         <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L4" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5"/>
       <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
       <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" t="s">
-        <v>24</v>
-      </c>
       <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6"/>
       <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
       <c r="I6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="J6" t="s">
-        <v>24</v>
-      </c>
       <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7"/>
       <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
       <c r="I7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
         <v>23</v>
       </c>
-      <c r="J7" t="s">
-        <v>24</v>
-      </c>
       <c r="K7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8"/>
       <c r="G8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
       <c r="I8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
         <v>23</v>
       </c>
-      <c r="J8" t="s">
-        <v>24</v>
-      </c>
       <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>